<commit_message>
avance semana 2 sprint 2
</commit_message>
<xml_diff>
--- a/burndown y trabajo de equipo/Boceto sprint 2.xlsx
+++ b/burndown y trabajo de equipo/Boceto sprint 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pato pobre\Documents\GitHub\SlimeSmasher\burndown y trabajo de equipo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CEAAB8-D403-45ED-8C9C-4D3AC650B1A9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93EF50EA-673A-4A3D-A7EB-64DE84311615}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="2430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="SPRINT 1 JEAN NAIL" sheetId="7" r:id="rId5"/>
     <sheet name="SPRINT 1 TRABAJO GRUPAL" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="53">
   <si>
     <t>SEMANA 1</t>
   </si>
@@ -172,6 +172,24 @@
   <si>
     <t>SPRINT 2</t>
   </si>
+  <si>
+    <t>arreglar colision arma</t>
+  </si>
+  <si>
+    <t>hacer union de enemigos</t>
+  </si>
+  <si>
+    <t>hacer particulado de nuevo con strpites conrrespondientes</t>
+  </si>
+  <si>
+    <t>arreglo de animacion[pendiente]</t>
+  </si>
+  <si>
+    <t>UI mas viva</t>
+  </si>
+  <si>
+    <t>IA Mesh</t>
+  </si>
 </sst>
 </file>
 
@@ -289,14 +307,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,8 +325,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -422,10 +440,10 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -462,7 +480,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -743,10 +761,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1070,10 +1088,10 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,10 +1742,10 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3527,8 +3545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8:P8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3537,20 +3555,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
@@ -3597,32 +3615,32 @@
       <c r="P5" s="8"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="10" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="9"/>
+      <c r="G6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="J6" s="15" t="s">
+      <c r="H6" s="9"/>
+      <c r="J6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="10" t="s">
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10" t="s">
+      <c r="N6" s="9"/>
+      <c r="O6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="10"/>
+      <c r="P6" s="9"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -3647,7 +3665,9 @@
         <v>5</v>
       </c>
       <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="O7" s="8">
+        <v>7</v>
+      </c>
       <c r="P7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
@@ -3673,20 +3693,20 @@
       <c r="P8" s="8"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
@@ -3721,36 +3741,36 @@
       <c r="P11" s="8"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10">
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
         <f>SUM(E7:F11)</f>
         <v>4</v>
       </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10">
+      <c r="F12" s="9"/>
+      <c r="G12" s="9">
         <f>SUM(G7:H11)</f>
         <v>4</v>
       </c>
-      <c r="H12" s="10"/>
-      <c r="J12" s="10" t="s">
+      <c r="H12" s="9"/>
+      <c r="J12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9">
         <f>SUM(M7:N11)</f>
         <v>5</v>
       </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10">
+      <c r="N12" s="9"/>
+      <c r="O12" s="9">
         <f>SUM(O7:P11)</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="10"/>
+        <v>7</v>
+      </c>
+      <c r="P12" s="9"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="12" t="s">
@@ -3762,14 +3782,14 @@
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="14"/>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
@@ -3801,19 +3821,19 @@
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="10" t="s">
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10" t="s">
+      <c r="F16" s="9"/>
+      <c r="G16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="10"/>
+      <c r="H16" s="9"/>
       <c r="J16" s="4" t="s">
         <v>9</v>
       </c>
@@ -3824,20 +3844,24 @@
         <v>11</v>
       </c>
       <c r="M16" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="N16" s="1">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="O16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8">
+        <v>5</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -3854,7 +3878,7 @@
         <v>5</v>
       </c>
       <c r="N17" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O17" s="1">
         <v>0</v>
@@ -3870,13 +3894,13 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="8"/>
@@ -3924,56 +3948,59 @@
       <c r="H24" s="8"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10">
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9">
         <f>SUM(E17:F24)</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10">
+        <v>5</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9">
         <f>SUM(G17:H24)</f>
         <v>0</v>
       </c>
-      <c r="H25" s="10"/>
+      <c r="H25" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="J14:O14"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G1:K2"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="K5:P5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="C5:H5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
@@ -3987,41 +4014,38 @@
     <mergeCell ref="O11:P11"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="M11:N11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="G1:K2"/>
-    <mergeCell ref="J4:P4"/>
-    <mergeCell ref="K5:P5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="C5:H5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="J14:O14"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4032,8 +4056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4043,20 +4067,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -4103,32 +4127,32 @@
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="J5" s="15" t="s">
+      <c r="H5" s="9"/>
+      <c r="J5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="10" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10" t="s">
+      <c r="N5" s="9"/>
+      <c r="O5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="10"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -4153,7 +4177,9 @@
         <v>5</v>
       </c>
       <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="O6" s="8">
+        <v>5</v>
+      </c>
       <c r="P6" s="8"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -4179,26 +4205,26 @@
       <c r="P7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <v>1</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9">
+      <c r="F8" s="9"/>
+      <c r="G8" s="10">
         <v>1</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -4239,36 +4265,36 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
         <f>SUM(E6:F10)</f>
         <v>6</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
         <f>SUM(G6:H10)</f>
         <v>10</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="J11" s="10" t="s">
+      <c r="H11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9">
         <f>SUM(M6:N10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10">
+      <c r="N11" s="9"/>
+      <c r="O11" s="9">
         <f>SUM(O6:P10)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="P11" s="9"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
@@ -4280,14 +4306,14 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -4319,19 +4345,19 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="10" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="9"/>
       <c r="J15" s="4" t="s">
         <v>9</v>
       </c>
@@ -4342,20 +4368,24 @@
         <v>5</v>
       </c>
       <c r="M15" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N15" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O15" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8">
+        <v>4</v>
+      </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -4379,22 +4409,26 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
@@ -4442,24 +4476,88 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9">
         <f>SUM(E16:F23)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10">
+        <v>5</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9">
         <f>SUM(G16:H23)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="10"/>
+      <c r="H24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="G1:K2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="J3:P3"/>
@@ -4476,70 +4574,6 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4550,8 +4584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4560,20 +4594,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -4620,32 +4654,32 @@
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="J5" s="15" t="s">
+      <c r="H5" s="9"/>
+      <c r="J5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="10" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10" t="s">
+      <c r="N5" s="9"/>
+      <c r="O5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="10"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -4670,7 +4704,9 @@
         <v>4</v>
       </c>
       <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="O6" s="8">
+        <v>2</v>
+      </c>
       <c r="P6" s="8"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -4696,30 +4732,38 @@
         <v>1</v>
       </c>
       <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
+      <c r="O7" s="8">
+        <v>1</v>
+      </c>
       <c r="P7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <v>0</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9">
+      <c r="F8" s="9"/>
+      <c r="G8" s="10">
         <v>2</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="J8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9">
+        <v>0</v>
+      </c>
+      <c r="N8" s="9"/>
+      <c r="O8" s="10">
+        <v>2</v>
+      </c>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
@@ -4754,36 +4798,36 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
         <f>SUM(E6:F10)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
         <f>SUM(G6:H10)</f>
         <v>7</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="J11" s="10" t="s">
+      <c r="H11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9">
         <f>SUM(M6:N10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10">
+      <c r="N11" s="9"/>
+      <c r="O11" s="9">
         <f>SUM(O6:P10)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="P11" s="9"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
@@ -4795,14 +4839,14 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -4834,19 +4878,19 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="10" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="9"/>
       <c r="J15" s="4" t="s">
         <v>9</v>
       </c>
@@ -4858,17 +4902,19 @@
         <v>8</v>
       </c>
       <c r="M15" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="N15" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O15" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
@@ -4904,13 +4950,13 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
@@ -4958,24 +5004,88 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9">
         <f>SUM(E16:F23)</f>
         <v>0</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10">
+      <c r="F24" s="9"/>
+      <c r="G24" s="9">
         <f>SUM(G16:H23)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="10"/>
+      <c r="H24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="G1:K2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="J3:P3"/>
@@ -4992,70 +5102,6 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5066,8 +5112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5076,20 +5122,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5136,32 +5182,32 @@
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="J5" s="15" t="s">
+      <c r="H5" s="9"/>
+      <c r="J5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="10" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10" t="s">
+      <c r="N5" s="9"/>
+      <c r="O5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="10"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -5186,7 +5232,9 @@
         <v>5</v>
       </c>
       <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="O6" s="8">
+        <v>5</v>
+      </c>
       <c r="P6" s="8"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -5212,26 +5260,26 @@
       <c r="P7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9">
         <v>1</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9">
+      <c r="F8" s="9"/>
+      <c r="G8" s="10">
         <v>1</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
@@ -5272,36 +5320,36 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
         <f>SUM(E6:F10)</f>
         <v>6</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
         <f>SUM(G6:H10)</f>
         <v>10</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="J11" s="10" t="s">
+      <c r="H11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9">
         <f>SUM(M6:N10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10">
+      <c r="N11" s="9"/>
+      <c r="O11" s="9">
         <f>SUM(O6:P10)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="P11" s="9"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
@@ -5313,14 +5361,14 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -5352,19 +5400,19 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="10" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="9"/>
       <c r="J15" s="4" t="s">
         <v>9</v>
       </c>
@@ -5382,14 +5430,18 @@
         <v>0</v>
       </c>
       <c r="O15" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>47</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8">
+        <v>4</v>
+      </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -5413,23 +5465,27 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8">
+        <v>1</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="J17" s="7"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
@@ -5477,24 +5533,88 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9">
         <f>SUM(E16:F23)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10">
+        <v>5</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9">
         <f>SUM(G16:H23)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="10"/>
+      <c r="H24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="G1:K2"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="J3:P3"/>
@@ -5511,70 +5631,6 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5585,27 +5641,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:P24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6:N6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
@@ -5652,32 +5708,32 @@
       <c r="P4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="J5" s="15" t="s">
+      <c r="H5" s="9"/>
+      <c r="J5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="10" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10" t="s">
+      <c r="N5" s="9"/>
+      <c r="O5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="10"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
@@ -5702,7 +5758,9 @@
         <v>5</v>
       </c>
       <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="O6" s="8">
+        <v>5</v>
+      </c>
       <c r="P6" s="8"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
@@ -5728,20 +5786,20 @@
       <c r="P7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="8"/>
@@ -5776,36 +5834,36 @@
       <c r="P10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
         <f>SUM(E6:F10)</f>
         <v>5</v>
       </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
         <f>SUM(G6:H10)</f>
         <v>5</v>
       </c>
-      <c r="H11" s="10"/>
-      <c r="J11" s="10" t="s">
+      <c r="H11" s="9"/>
+      <c r="J11" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9">
         <f>SUM(M6:N10)</f>
         <v>5</v>
       </c>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10">
+      <c r="N11" s="9"/>
+      <c r="O11" s="9">
         <f>SUM(O6:P10)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="10"/>
+        <v>5</v>
+      </c>
+      <c r="P11" s="9"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13" s="12" t="s">
@@ -5817,14 +5875,14 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="14"/>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
@@ -5856,19 +5914,19 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="10" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="10"/>
+      <c r="H15" s="9"/>
       <c r="J15" s="4" t="s">
         <v>9</v>
       </c>
@@ -5880,10 +5938,10 @@
         <v>10</v>
       </c>
       <c r="M15" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="N15" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O15" s="1">
         <v>0</v>
@@ -5917,22 +5975,26 @@
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="8"/>
+      <c r="B17" s="8" t="s">
+        <v>52</v>
+      </c>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8">
+        <v>5</v>
+      </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
@@ -5980,24 +6042,88 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10">
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9">
         <f>SUM(E16:F23)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10">
+        <v>5</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9">
         <f>SUM(G16:H23)</f>
         <v>0</v>
       </c>
-      <c r="H24" s="10"/>
+      <c r="H24" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="C14:H14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="M7:N7"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="J3:P3"/>
     <mergeCell ref="G1:K2"/>
@@ -6014,70 +6140,6 @@
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:N11"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="C14:H14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6100,49 +6162,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="2:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="L4" s="10" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="L4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="10"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="4" t="s">
         <v>24</v>
       </c>
@@ -6150,20 +6212,20 @@
         <v>9</v>
       </c>
       <c r="F5" s="3"/>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="10"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="4" t="s">
         <v>24</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="9"/>
       <c r="N5" s="4" t="s">
         <v>24</v>
       </c>
@@ -6205,10 +6267,10 @@
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="1">
         <v>25</v>
       </c>
@@ -6216,20 +6278,20 @@
         <v>36</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="9"/>
       <c r="I7" s="1">
         <v>25</v>
       </c>
       <c r="J7" s="1">
         <v>0</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="9"/>
       <c r="N7" s="1">
         <v>25</v>
       </c>
@@ -6246,11 +6308,11 @@
       <c r="E9" s="13"/>
       <c r="F9" s="14"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
@@ -6267,10 +6329,10 @@
         <v>20</v>
       </c>
       <c r="H10" s="3"/>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="10"/>
+      <c r="J10" s="9"/>
       <c r="K10" s="1">
         <v>75</v>
       </c>
@@ -6292,10 +6354,10 @@
         <v>39</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="10"/>
+      <c r="J11" s="9"/>
       <c r="K11" s="1">
         <f>E7+J7+O7</f>
         <v>36</v>
@@ -6318,26 +6380,16 @@
         <v>0</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="10"/>
+      <c r="J12" s="9"/>
       <c r="K12" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="F1:K2"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
@@ -6346,6 +6398,16 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="F1:K2"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>